<commit_message>
Cauchy fitting, changed conversion constant for verdet
</commit_message>
<xml_diff>
--- a/boundary/data/angle_data.xlsx
+++ b/boundary/data/angle_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackson\physics_387\boundary\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99875414-6167-4296-B26D-538231FE89D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120F4CEE-BFB2-4B5A-8AFD-5D9E857AADE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{951BB4D2-3E14-4958-B323-453993576732}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{951BB4D2-3E14-4958-B323-453993576732}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Thick boi</t>
   </si>
@@ -47,15 +47,59 @@
     <t>Eye found Brewster's angle w/ p polarized light</t>
   </si>
   <si>
-    <t>TIR Angles</t>
+    <t>Brewster's angle with S polarized light</t>
+  </si>
+  <si>
+    <t>None Found</t>
+  </si>
+  <si>
+    <t>TIR Angle for p polarized</t>
+  </si>
+  <si>
+    <t>TIR for S polarized</t>
+  </si>
+  <si>
+    <t>Part 2</t>
+  </si>
+  <si>
+    <t>Incident angle to normal</t>
+  </si>
+  <si>
+    <t>Thick boi, air to glass</t>
+  </si>
+  <si>
+    <t>Turquoise boi, air to glass</t>
+  </si>
+  <si>
+    <t>Refracted goniometer angle (+/-0.5)</t>
+  </si>
+  <si>
+    <t>Refracted angle to beam</t>
+  </si>
+  <si>
+    <t>Turquoise boi, glass to air</t>
+  </si>
+  <si>
+    <t>Incident Goniometer angle (+/-0.5)</t>
+  </si>
+  <si>
+    <t>Thick boi, glass to air</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,8 +127,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,27 +444,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBADA283-CCC7-4ED7-A7A3-F4C09541EAA1}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="50.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -429,8 +483,14 @@
       <c r="C2">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -439,6 +499,497 @@
       </c>
       <c r="C3">
         <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <v>180</v>
+      </c>
+      <c r="D8">
+        <f>90-B8</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>180-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <v>176</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:D17" si="0">90-B9</f>
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:E16" si="1">180-C9</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <v>172.5</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>168</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>164</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>40</v>
+      </c>
+      <c r="C13">
+        <v>160</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>154.5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>148</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>140</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>90</v>
+      </c>
+      <c r="C19">
+        <v>180</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19" si="2">90-B19</f>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19" si="3">180-C19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>80</v>
+      </c>
+      <c r="C20">
+        <v>174.5</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:D23" si="4">90-B20</f>
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20:E23" si="5">180-C20</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>70</v>
+      </c>
+      <c r="C21">
+        <v>169.5</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="5"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>60</v>
+      </c>
+      <c r="C22">
+        <v>161</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>50</v>
+      </c>
+      <c r="C23">
+        <v>145</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>90</v>
+      </c>
+      <c r="C25">
+        <v>180</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25" si="6">90-B25</f>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ref="E25" si="7">180-C25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>80</v>
+      </c>
+      <c r="C26">
+        <v>176.5</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:E35" si="8">90-B26</f>
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26:E35" si="9">180-C26</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>70</v>
+      </c>
+      <c r="C27">
+        <v>173.5</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="9"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>60</v>
+      </c>
+      <c r="C28">
+        <v>170</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>165.5</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="9"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>40</v>
+      </c>
+      <c r="C30">
+        <v>161.5</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="9"/>
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>156</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>149.5</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="9"/>
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>142</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="8"/>
+        <v>80</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35">
+        <v>90</v>
+      </c>
+      <c r="C35">
+        <v>180</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>80</v>
+      </c>
+      <c r="C36">
+        <v>175</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ref="D36:D39" si="10">90-B36</f>
+        <v>10</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ref="E36:E39" si="11">180-C36</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>70</v>
+      </c>
+      <c r="C37">
+        <v>169</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="11"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>60</v>
+      </c>
+      <c r="C38">
+        <v>163</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="11"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>50</v>
+      </c>
+      <c r="C39">
+        <v>147.5</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="11"/>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>